<commit_message>
further optimizations. added a* search to benchmarker
</commit_message>
<xml_diff>
--- a/src/data/ips_profile.xlsx
+++ b/src/data/ips_profile.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SuhasVittal/Documents/programming/qcr/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5ECE57C4-C87D-8440-A039-03458F76106A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411953AF-AD86-554D-B18C-4F74121B880A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1060" windowWidth="27240" windowHeight="16440"/>
+    <workbookView xWindow="1180" yWindow="1060" windowWidth="27240" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ips_profile" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
   <si>
     <t>size</t>
   </si>
@@ -227,12 +227,90 @@
   </si>
   <si>
     <t>4gt4-v0_72.qasm</t>
+  </si>
+  <si>
+    <t>SUMMARY OUTPUT</t>
+  </si>
+  <si>
+    <t>Regression Statistics</t>
+  </si>
+  <si>
+    <t>Multiple R</t>
+  </si>
+  <si>
+    <t>R Square</t>
+  </si>
+  <si>
+    <t>Adjusted R Square</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Significance F</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Lower 95%</t>
+  </si>
+  <si>
+    <t>Upper 95%</t>
+  </si>
+  <si>
+    <t>Lower 95.0%</t>
+  </si>
+  <si>
+    <t>Upper 95.0%</t>
+  </si>
+  <si>
+    <t>X Variable 1</t>
+  </si>
+  <si>
+    <t>X Variable 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1102,16 +1180,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1133,8 +1211,20 @@
       <c r="H1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1159,8 +1249,17 @@
       <c r="H2">
         <v>0.107142857142857</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="K2">
+        <v>2.9841269841269802</v>
+      </c>
+      <c r="L2">
+        <v>0.107142857142857</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1185,8 +1284,21 @@
       <c r="H3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>0.78734622144112398</v>
+      </c>
+      <c r="K3">
+        <v>4.3956422018348604</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="O3" s="4"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1211,10 +1323,23 @@
       <c r="H4">
         <v>2.6086956521739101E-2</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>0.77647058823529402</v>
+      </c>
+      <c r="K4">
+        <v>3.0706806282722501</v>
+      </c>
+      <c r="L4">
+        <v>2.6086956521739101E-2</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0.84453830586836176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1239,10 +1364,23 @@
       <c r="H5">
         <v>-4.2826552462526701E-2</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>0.78888265019651804</v>
+      </c>
+      <c r="K5">
+        <v>7.4120437956204297</v>
+      </c>
+      <c r="L5">
+        <v>-4.2826552462526701E-2</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0.71324495007900257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1267,10 +1405,23 @@
       <c r="H6">
         <v>2.3809523809523801E-2</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>0.77227722772277196</v>
+      </c>
+      <c r="K6">
+        <v>3.0612244897959102</v>
+      </c>
+      <c r="L6">
+        <v>2.3809523809523801E-2</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0.70221590969742576</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1295,10 +1446,23 @@
       <c r="H7">
         <v>0</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>0.810276679841897</v>
+      </c>
+      <c r="K7">
+        <v>4.0609137055837499</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O7" s="1">
+        <v>6.9259204475935851E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1323,10 +1487,23 @@
       <c r="H8">
         <v>-6.5573770491803199E-2</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>6.4535519125683001</v>
+      </c>
+      <c r="L8">
+        <v>-6.5573770491803199E-2</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O8" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1351,10 +1528,17 @@
       <c r="H9">
         <v>2.5179856115107899E-2</v>
       </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <v>0.81692913385826704</v>
+      </c>
+      <c r="K9">
+        <v>5.11625</v>
+      </c>
+      <c r="L9">
+        <v>2.5179856115107899E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1379,8 +1563,20 @@
       <c r="H10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>2.9098712446351902</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="N10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1405,8 +1601,33 @@
       <c r="H11">
         <v>4.4247787610619399E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>0.77433628318584002</v>
+      </c>
+      <c r="K11">
+        <v>3.7529761904761898</v>
+      </c>
+      <c r="L11">
+        <v>4.4247787610619399E-2</v>
+      </c>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="S11" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1431,14 +1652,35 @@
       <c r="H12">
         <v>1.3357079252003501E-2</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>0.81457313757476801</v>
+      </c>
+      <c r="K12">
+        <v>7.3015437392795803</v>
+      </c>
+      <c r="L12">
+        <v>1.3357079252003501E-2</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O12" s="1">
+        <v>2</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0.62042026084594648</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>0.31021013042297324</v>
+      </c>
+      <c r="R12" s="1">
+        <v>64.669719703848742</v>
+      </c>
+      <c r="S12" s="1">
+        <v>7.8575643287134505E-15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1463,14 +1705,31 @@
       <c r="H13">
         <v>1.3698630136986301E-2</v>
       </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <v>0.77777777777777701</v>
+      </c>
+      <c r="K13">
+        <v>3.0946502057613099</v>
+      </c>
+      <c r="L13">
+        <v>1.3698630136986301E-2</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O13" s="1">
+        <v>52</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0.24943554504125356</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>4.796837404639492E-3</v>
+      </c>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+    </row>
+    <row r="14" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1495,14 +1754,29 @@
       <c r="H14">
         <v>-2.0134228187919399E-2</v>
       </c>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-    </row>
-    <row r="15" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>0.78245614035087696</v>
+      </c>
+      <c r="K14">
+        <v>3.73781902552204</v>
+      </c>
+      <c r="L14">
+        <v>-2.0134228187919399E-2</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="O14" s="2">
+        <v>54</v>
+      </c>
+      <c r="P14" s="2">
+        <v>0.86985580588720002</v>
+      </c>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+    </row>
+    <row r="15" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1527,14 +1801,17 @@
       <c r="H15">
         <v>-5.6338028169014003E-2</v>
       </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J15">
+        <v>0.76628352490421403</v>
+      </c>
+      <c r="K15">
+        <v>4.4571428571428502</v>
+      </c>
+      <c r="L15">
+        <v>-5.6338028169014003E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1559,8 +1836,42 @@
       <c r="H16">
         <v>3.3266129032258E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J16">
+        <v>0.81690997566909895</v>
+      </c>
+      <c r="K16">
+        <v>5.7672644028996496</v>
+      </c>
+      <c r="L16">
+        <v>3.3266129032258E-2</v>
+      </c>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="T16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="U16" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1585,8 +1896,44 @@
       <c r="H17">
         <v>0.18348623853210999</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J17">
+        <v>0.83976261127596397</v>
+      </c>
+      <c r="K17">
+        <v>4.3076923076923004</v>
+      </c>
+      <c r="L17">
+        <v>0.18348623853210999</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O17" s="1">
+        <v>0.48303430492221033</v>
+      </c>
+      <c r="P17" s="1">
+        <v>5.831599770555481E-2</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>8.2830496592224048</v>
+      </c>
+      <c r="R17" s="1">
+        <v>4.5569020800347863E-11</v>
+      </c>
+      <c r="S17" s="1">
+        <v>0.36601469444237417</v>
+      </c>
+      <c r="T17" s="1">
+        <v>0.60005391540204656</v>
+      </c>
+      <c r="U17" s="1">
+        <v>0.36601469444237417</v>
+      </c>
+      <c r="V17" s="1">
+        <v>0.60005391540204656</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1611,8 +1958,44 @@
       <c r="H18">
         <v>6.6666666666666596E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J18">
+        <v>0.91111111111111098</v>
+      </c>
+      <c r="K18">
+        <v>2.7489177489177399</v>
+      </c>
+      <c r="L18">
+        <v>6.6666666666666596E-2</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="O18" s="1">
+        <v>-0.50017410943110707</v>
+      </c>
+      <c r="P18" s="1">
+        <v>4.4617460694801638E-2</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>-11.210277358733284</v>
+      </c>
+      <c r="R18" s="1">
+        <v>1.7372920621327276E-15</v>
+      </c>
+      <c r="S18" s="1">
+        <v>-0.58970559438429615</v>
+      </c>
+      <c r="T18" s="1">
+        <v>-0.41064262447791799</v>
+      </c>
+      <c r="U18" s="1">
+        <v>-0.58970559438429615</v>
+      </c>
+      <c r="V18" s="1">
+        <v>-0.41064262447791799</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1637,8 +2020,44 @@
       <c r="H19">
         <v>5.6198347107437999E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J19">
+        <v>0.80250481695568399</v>
+      </c>
+      <c r="K19">
+        <v>6.5872420262664102</v>
+      </c>
+      <c r="L19">
+        <v>5.6198347107437999E-2</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="O19" s="2">
+        <v>-1.5109659454523944E-2</v>
+      </c>
+      <c r="P19" s="2">
+        <v>7.9318895349467164E-3</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>-1.9049256029037027</v>
+      </c>
+      <c r="R19" s="2">
+        <v>6.2327134990827239E-2</v>
+      </c>
+      <c r="S19" s="2">
+        <v>-3.1026160247926995E-2</v>
+      </c>
+      <c r="T19" s="2">
+        <v>8.0684133887910792E-4</v>
+      </c>
+      <c r="U19" s="2">
+        <v>-3.1026160247926995E-2</v>
+      </c>
+      <c r="V19" s="2">
+        <v>8.0684133887910792E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1663,8 +2082,17 @@
       <c r="H20">
         <v>2.3255813953488299E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J20">
+        <v>0.78421052631578902</v>
+      </c>
+      <c r="K20">
+        <v>3.5674740484429002</v>
+      </c>
+      <c r="L20">
+        <v>2.3255813953488299E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1689,8 +2117,17 @@
       <c r="H21">
         <v>6.8965517241379301E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J21">
+        <v>0.79139072847682101</v>
+      </c>
+      <c r="K21">
+        <v>3.6673866090712699</v>
+      </c>
+      <c r="L21">
+        <v>6.8965517241379301E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1715,8 +2152,17 @@
       <c r="H22">
         <v>-1.7094017094016999E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J22">
+        <v>0.78087649402390402</v>
+      </c>
+      <c r="K22">
+        <v>3.5661375661375598</v>
+      </c>
+      <c r="L22">
+        <v>-1.7094017094016999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1741,8 +2187,17 @@
       <c r="H23">
         <v>4.0178571428571397E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J23">
+        <v>0.77241379310344804</v>
+      </c>
+      <c r="K23">
+        <v>3.8366718027734898</v>
+      </c>
+      <c r="L23">
+        <v>4.0178571428571397E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1767,8 +2222,17 @@
       <c r="H24">
         <v>1.7142857142857099E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J24">
+        <v>0.82021276595744597</v>
+      </c>
+      <c r="K24">
+        <v>5.5650708024275097</v>
+      </c>
+      <c r="L24">
+        <v>1.7142857142857099E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1793,8 +2257,17 @@
       <c r="H25">
         <v>-3.38983050847457E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J25">
+        <v>0.76923076923076905</v>
+      </c>
+      <c r="K25">
+        <v>3.5263157894736801</v>
+      </c>
+      <c r="L25">
+        <v>-3.38983050847457E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1819,8 +2292,17 @@
       <c r="H26">
         <v>3.6608863198458498E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J26">
+        <v>0.82021276595744597</v>
+      </c>
+      <c r="K26">
+        <v>5.5650708024275097</v>
+      </c>
+      <c r="L26">
+        <v>3.6608863198458498E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1845,8 +2327,17 @@
       <c r="H27">
         <v>6.4516129032257993E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J27">
+        <v>0.77697841726618699</v>
+      </c>
+      <c r="K27">
+        <v>3.0436893203883399</v>
+      </c>
+      <c r="L27">
+        <v>6.4516129032257993E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1871,8 +2362,17 @@
       <c r="H28">
         <v>-3.8461538461538401E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J28">
+        <v>0.79629629629629595</v>
+      </c>
+      <c r="K28">
+        <v>3.2546583850931601</v>
+      </c>
+      <c r="L28">
+        <v>-3.8461538461538401E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1897,8 +2397,17 @@
       <c r="H29">
         <v>3.4482758620689599E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J29">
+        <v>0.79545454545454497</v>
+      </c>
+      <c r="K29">
+        <v>3.5204081632653001</v>
+      </c>
+      <c r="L29">
+        <v>3.4482758620689599E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -1923,8 +2432,17 @@
       <c r="H30">
         <v>3.7037037037037E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J30">
+        <v>0.78217821782178198</v>
+      </c>
+      <c r="K30">
+        <v>3.4093959731543602</v>
+      </c>
+      <c r="L30">
+        <v>3.7037037037037E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -1949,8 +2467,17 @@
       <c r="H31">
         <v>-2.04081632653061E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J31">
+        <v>0.78756476683937804</v>
+      </c>
+      <c r="K31">
+        <v>3.70547945205479</v>
+      </c>
+      <c r="L31">
+        <v>-2.04081632653061E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -1975,8 +2502,17 @@
       <c r="H32">
         <v>0.13793103448275801</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J32">
+        <v>0.79850746268656703</v>
+      </c>
+      <c r="K32">
+        <v>2.91625615763546</v>
+      </c>
+      <c r="L32">
+        <v>0.13793103448275801</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -2001,8 +2537,17 @@
       <c r="H33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J33">
+        <v>0.77272727272727204</v>
+      </c>
+      <c r="K33">
+        <v>3.5657894736842102</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -2027,8 +2572,17 @@
       <c r="H34">
         <v>2.9850746268656699E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J34">
+        <v>0.85496183206106802</v>
+      </c>
+      <c r="K34">
+        <v>3.5</v>
+      </c>
+      <c r="L34">
+        <v>2.9850746268656699E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -2053,8 +2607,17 @@
       <c r="H35">
         <v>-1.47058823529411E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J35">
+        <v>0.85925925925925895</v>
+      </c>
+      <c r="K35">
+        <v>3.4470046082949302</v>
+      </c>
+      <c r="L35">
+        <v>-1.47058823529411E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -2079,8 +2642,17 @@
       <c r="H36">
         <v>2.5510204081632602E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J36">
+        <v>0.77064220183486198</v>
+      </c>
+      <c r="K36">
+        <v>3.82561728395061</v>
+      </c>
+      <c r="L36">
+        <v>2.5510204081632602E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -2105,8 +2677,17 @@
       <c r="H37">
         <v>-0.10691823899371</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J37">
+        <v>0.77616279069767402</v>
+      </c>
+      <c r="K37">
+        <v>4.3087378640776697</v>
+      </c>
+      <c r="L37">
+        <v>-0.10691823899371</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -2131,8 +2712,17 @@
       <c r="H38">
         <v>3.5422343324250601E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J38">
+        <v>0.78891820580474903</v>
+      </c>
+      <c r="K38">
+        <v>3.7517123287671201</v>
+      </c>
+      <c r="L38">
+        <v>3.5422343324250601E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -2157,8 +2747,17 @@
       <c r="H39">
         <v>4.5977011494252797E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J39">
+        <v>0.80540540540540495</v>
+      </c>
+      <c r="K39">
+        <v>3.58007117437722</v>
+      </c>
+      <c r="L39">
+        <v>4.5977011494252797E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -2183,8 +2782,17 @@
       <c r="H40">
         <v>1.20481927710843E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J40">
+        <v>0.84276729559748398</v>
+      </c>
+      <c r="K40">
+        <v>3.8588235294117599</v>
+      </c>
+      <c r="L40">
+        <v>1.20481927710843E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -2209,8 +2817,17 @@
       <c r="H41">
         <v>-0.121037463976945</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J41">
+        <v>0.77777777777777701</v>
+      </c>
+      <c r="K41">
+        <v>4.6274319066147802</v>
+      </c>
+      <c r="L41">
+        <v>-0.121037463976945</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -2235,8 +2852,17 @@
       <c r="H42">
         <v>7.4866310160427801E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J42">
+        <v>0.79213483146067398</v>
+      </c>
+      <c r="K42">
+        <v>4.7895699908508602</v>
+      </c>
+      <c r="L42">
+        <v>7.4866310160427801E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -2261,8 +2887,17 @@
       <c r="H43">
         <v>-9.5315024232633203E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J43">
+        <v>0.82840800762630995</v>
+      </c>
+      <c r="K43">
+        <v>5.9742976688583296</v>
+      </c>
+      <c r="L43">
+        <v>-9.5315024232633203E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -2287,8 +2922,17 @@
       <c r="H44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J44">
+        <v>0.79562043795620396</v>
+      </c>
+      <c r="K44">
+        <v>3.7438423645320098</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -2313,8 +2957,17 @@
       <c r="H45">
         <v>2.9702970297029702E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J45">
+        <v>0.78854625550660795</v>
+      </c>
+      <c r="K45">
+        <v>3.66374269005847</v>
+      </c>
+      <c r="L45">
+        <v>2.9702970297029702E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>51</v>
       </c>
@@ -2339,8 +2992,17 @@
       <c r="H46">
         <v>2.7397260273972601E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J46">
+        <v>0.78527607361963103</v>
+      </c>
+      <c r="K46">
+        <v>3.1538461538461502</v>
+      </c>
+      <c r="L46">
+        <v>2.7397260273972601E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -2365,8 +3027,17 @@
       <c r="H47">
         <v>-5.8823529411764698E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J47">
+        <v>1.4</v>
+      </c>
+      <c r="K47">
+        <v>2.29720279720279</v>
+      </c>
+      <c r="L47">
+        <v>-5.8823529411764698E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -2391,8 +3062,17 @@
       <c r="H48">
         <v>5.8823529411764698E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J48">
+        <v>0.78592814371257402</v>
+      </c>
+      <c r="K48">
+        <v>4.98519249753208</v>
+      </c>
+      <c r="L48">
+        <v>5.8823529411764698E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>54</v>
       </c>
@@ -2417,8 +3097,17 @@
       <c r="H49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J49">
+        <v>1.16535433070866</v>
+      </c>
+      <c r="K49">
+        <v>2.2527075812274302</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>55</v>
       </c>
@@ -2443,8 +3132,17 @@
       <c r="H50">
         <v>-0.84297520661156999</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J50">
+        <v>2.2857142857142798</v>
+      </c>
+      <c r="K50">
+        <v>1.8168604651162701</v>
+      </c>
+      <c r="L50">
+        <v>-0.84297520661156999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -2469,8 +3167,17 @@
       <c r="H51">
         <v>-3.9370078740157403E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J51">
+        <v>1.02870813397129</v>
+      </c>
+      <c r="K51">
+        <v>2.7054455445544501</v>
+      </c>
+      <c r="L51">
+        <v>-3.9370078740157403E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>57</v>
       </c>
@@ -2495,8 +3202,17 @@
       <c r="H52">
         <v>-3.1779661016949103E-2</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J52">
+        <v>0.79204339963833603</v>
+      </c>
+      <c r="K52">
+        <v>6.9910015649452202</v>
+      </c>
+      <c r="L52">
+        <v>-3.1779661016949103E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>58</v>
       </c>
@@ -2521,8 +3237,17 @@
       <c r="H53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J53">
+        <v>0.77464788732394296</v>
+      </c>
+      <c r="K53">
+        <v>4.3007518796992397</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>59</v>
       </c>
@@ -2547,8 +3272,17 @@
       <c r="H54">
         <v>-5.2631578947368397E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J54">
+        <v>0.83073929961089499</v>
+      </c>
+      <c r="K54">
+        <v>4.73600973236009</v>
+      </c>
+      <c r="L54">
+        <v>-5.2631578947368397E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -2573,8 +3307,17 @@
       <c r="H55">
         <v>-2.0134228187919399E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J55">
+        <v>0.78287461773700295</v>
+      </c>
+      <c r="K55">
+        <v>4.3428571428571399</v>
+      </c>
+      <c r="L55">
+        <v>-2.0134228187919399E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -2597,6 +3340,15 @@
         <v>5.0555651271125299</v>
       </c>
       <c r="H56">
+        <v>1.51515151515151E-2</v>
+      </c>
+      <c r="J56">
+        <v>0.82481751824817495</v>
+      </c>
+      <c r="K56">
+        <v>3.3644859813084098</v>
+      </c>
+      <c r="L56">
         <v>1.51515151515151E-2</v>
       </c>
     </row>

</xml_diff>